<commit_message>
eligable for dispatch logic fix
eligable for dispatch logic fix
</commit_message>
<xml_diff>
--- a/1 MALL 2024 Faktura till kattägare (1 katt) 240101-01 Misse.xlsx
+++ b/1 MALL 2024 Faktura till kattägare (1 katt) 240101-01 Misse.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Blad1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Fakturadatum</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-10-23</t>
+    <t xml:space="preserve">241027</t>
   </si>
   <si>
     <t xml:space="preserve">151 50 Enhörna</t>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Förfallodatum</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-11-27</t>
+    <t xml:space="preserve">241127</t>
   </si>
   <si>
     <t xml:space="preserve">info@lohaga.se</t>
@@ -406,121 +406,15 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>